<commit_message>
deleted git ignore file
</commit_message>
<xml_diff>
--- a/data/Screenshot.xlsx
+++ b/data/Screenshot.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32">
   <si>
     <t>imagename</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>https://dashboard-test.kommunicate.io/helpcenter/content</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>https://dashboard-test.kommunicate.io/helpcenter/answer-bot</t>
   </si>
   <si>
     <t>test step</t>
@@ -113,9 +119,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
@@ -143,6 +149,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -153,6 +181,97 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -165,119 +284,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -294,6 +300,132 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -312,169 +444,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -493,6 +499,56 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -535,200 +591,150 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1112,13 +1118,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="7" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="12.75" customWidth="1"/>
   </cols>
@@ -1185,6 +1191,14 @@
       </c>
       <c r="B8" s="2" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1196,6 +1210,7 @@
     <hyperlink ref="B6" r:id="rId5" display="https://dashboard-test.kommunicate.io/bots/bot-integrations"/>
     <hyperlink ref="B7" r:id="rId6" display="https://dashboard-test.kommunicate.io/integrations"/>
     <hyperlink ref="B8" r:id="rId7" display="https://dashboard-test.kommunicate.io/helpcenter/content"/>
+    <hyperlink ref="B9" r:id="rId8" display="https://dashboard-test.kommunicate.io/helpcenter/answer-bot"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
@@ -1218,83 +1233,83 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" t="s">
-        <v>23</v>
-      </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>5</v>
@@ -1302,16 +1317,16 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>